<commit_message>
solicitud graficas  -Guion 1-Grados 8 y 9
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/EsqueletoGuion_CS_09_01_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion01/EsqueletoGuion_CS_09_01_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9255" tabRatio="729"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9255" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -302,7 +302,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,26 +364,12 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Cambria"/>
       <family val="1"/>
@@ -402,12 +388,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -421,14 +401,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,12 +424,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -479,12 +452,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -492,12 +459,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -980,7 +941,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1008,117 +969,69 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1791,7 +1704,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1801,7 +1714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1815,7 +1728,7 @@
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="17" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1831,7 +1744,7 @@
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="18" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1911,22 +1824,22 @@
       </c>
     </row>
     <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="62" t="s">
+      <c r="C2" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F2" s="27">
+      <c r="F2" s="19">
         <v>1</v>
       </c>
       <c r="G2"/>
@@ -1937,22 +1850,22 @@
       <c r="L2"/>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" s="62" t="s">
+      <c r="C3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="19">
         <v>2</v>
       </c>
       <c r="G3"/>
@@ -1963,326 +1876,326 @@
       <c r="L3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="63" t="s">
+      <c r="C4" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="19">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="63" t="s">
+      <c r="C5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="20">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="62" t="s">
+      <c r="C6" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="19">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="63" t="s">
+      <c r="C7" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="19">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="63" t="s">
+      <c r="C8" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="19">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="62" t="s">
+      <c r="C9" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="62" t="s">
+      <c r="E9" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="19">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="27" t="s">
+      <c r="C10" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="19">
         <v>11</v>
       </c>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="27" t="s">
+      <c r="C11" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="19">
         <v>12</v>
       </c>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="27" t="s">
+      <c r="C12" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="19">
         <v>13</v>
       </c>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="27" t="s">
+      <c r="C13" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="19">
         <v>14</v>
       </c>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="27" t="s">
+      <c r="C14" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="19">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="27" t="s">
+      <c r="C15" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="19">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="27" t="s">
+      <c r="C16" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="19">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="27" t="s">
+      <c r="C17" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="19">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="27" t="s">
+      <c r="C18" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="27" t="s">
+      <c r="E18" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="19">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="27" t="s">
+      <c r="C19" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="19">
         <v>22</v>
       </c>
     </row>
@@ -2446,7 +2359,7 @@
       <c r="A4" s="14">
         <v>3</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="19" t="s">
         <v>40</v>
       </c>
       <c r="C4" s="14" t="s">
@@ -2457,7 +2370,7 @@
       <c r="A5" s="14">
         <v>4</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="19" t="s">
         <v>43</v>
       </c>
       <c r="C5" s="14" t="s">
@@ -2663,79 +2576,79 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="61"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="59"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="29"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="55"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="59"/>
+      <c r="A25" s="28"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="29"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="55"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="59"/>
+      <c r="A26" s="28"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="29"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="55"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="59"/>
+      <c r="A27" s="28"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="29"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="55"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="59"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="29"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="55"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="59"/>
+      <c r="A29" s="28"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="29"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="55"/>
-      <c r="B30" s="55"/>
-      <c r="C30" s="59"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="29"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="55"/>
-      <c r="B31" s="55"/>
-      <c r="C31" s="59"/>
+      <c r="A31" s="28"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="29"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="55"/>
-      <c r="B32" s="55"/>
-      <c r="C32" s="59"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="29"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="55"/>
-      <c r="B33" s="55"/>
-      <c r="C33" s="59"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="29"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="55"/>
-      <c r="B34" s="55"/>
-      <c r="C34" s="59"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="29"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="55"/>
-      <c r="B35" s="55"/>
-      <c r="C35" s="59"/>
+      <c r="A35" s="28"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="29"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="59"/>
-      <c r="B36" s="59"/>
-      <c r="C36" s="60"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="30"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="59"/>
-      <c r="B37" s="59"/>
-      <c r="C37" s="60"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="30"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="59"/>
-      <c r="B38" s="59"/>
-      <c r="C38" s="60"/>
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="30"/>
     </row>
   </sheetData>
   <sortState ref="A2:C38">
@@ -2756,13 +2669,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26" style="45" customWidth="1"/>
+    <col min="1" max="1" width="26" style="27" customWidth="1"/>
     <col min="2" max="2" width="42.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
@@ -2772,1274 +2685,1322 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="35" t="s">
         <v>4</v>
       </c>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="31" t="s">
+      <c r="A2" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="31" t="s">
+      <c r="A3" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="14" t="s">
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="31" t="s">
+      <c r="A4" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="31"/>
-      <c r="C5" s="30" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="69"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="14" t="s">
+      <c r="D5" s="41"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="I5" s="14"/>
-      <c r="J5">
+      <c r="I5" s="36"/>
+      <c r="J5" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="31" t="s">
+    <row r="6" spans="1:10" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="58"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="35" t="s">
+      <c r="D6" s="42"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="I6" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J6" s="37">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="32" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="31" t="s">
+    <row r="7" spans="1:10" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="35" t="s">
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="35" t="s">
+      <c r="I7" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="32">
+      <c r="J7" s="37">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="65" t="s">
+      <c r="A8" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="40"/>
-      <c r="I8" s="34"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="65" t="s">
+      <c r="A9" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="36"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="65" t="s">
+      <c r="A10" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="57"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="65" t="s">
+      <c r="A11" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="17"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="13" t="s">
+      <c r="D11" s="22"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="31" t="s">
+      <c r="A12" s="25"/>
+      <c r="B12" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="17"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="31" t="s">
+      <c r="A13" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="54" t="s">
+      <c r="C13" s="44"/>
+      <c r="D13" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="31" t="s">
+      <c r="A14" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="36" t="s">
+      <c r="C14" s="44"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="31" t="s">
+      <c r="A15" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="34" t="s">
+      <c r="C15" s="44"/>
+      <c r="D15" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="E15" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="31" t="s">
+      <c r="A16" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="36" t="s">
+      <c r="C16" s="44"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="40" t="s">
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="I16" s="35" t="s">
+      <c r="I16" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" s="31" t="s">
+      <c r="A17" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="42" t="s">
+      <c r="C17" s="38"/>
+      <c r="D17" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="E17" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="42"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="31" t="s">
+      <c r="A18" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="16" t="s">
+      <c r="C18" s="38"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" s="31" t="s">
+      <c r="A19" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16" t="s">
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="31" t="s">
+      <c r="A20" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16" t="s">
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16" t="s">
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="I20" s="16" t="s">
+      <c r="I20" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="31" t="s">
+      <c r="A21" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16" t="s">
+      <c r="C21" s="38"/>
+      <c r="D21" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="31" t="s">
+      <c r="A22" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="16" t="s">
+      <c r="C22" s="38"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="31" t="s">
+      <c r="A23" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="16" t="s">
+      <c r="C23" s="38"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16" t="s">
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="I23" s="16" t="s">
+      <c r="I23" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="2">
         <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="31" t="s">
+      <c r="A24" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="47"/>
-      <c r="E24" s="46" t="s">
+      <c r="C24" s="38"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46" t="s">
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="I24" s="46" t="s">
+      <c r="I24" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="2">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="64" t="s">
+      <c r="A25" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="47"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="64" t="s">
+      <c r="A26" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="46" t="s">
+      <c r="C26" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="D26" s="48"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="64" t="s">
+      <c r="A27" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="46" t="s">
+      <c r="C27" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="47"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="46"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="38"/>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="64" t="s">
+      <c r="A28" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C28" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="D28" s="29"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19" t="s">
+      <c r="D28" s="42"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="I28" s="19" t="s">
+      <c r="I28" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="2">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" s="31" t="s">
+      <c r="A29" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="19" t="s">
+      <c r="C29" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30" s="31" t="s">
+      <c r="A30" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C30" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="20"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19" t="s">
+      <c r="D30" s="45"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="I30" s="19" t="s">
+      <c r="I30" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="2">
         <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="31" t="s">
+      <c r="A31" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="20" t="s">
+      <c r="C31" s="38"/>
+      <c r="D31" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="E31" s="49" t="s">
+      <c r="E31" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="19"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B32" s="31" t="s">
+      <c r="A32" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="19" t="s">
+      <c r="C32" s="38"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="31" t="s">
+      <c r="A33" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19" t="s">
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="G33" s="19" t="s">
+      <c r="G33" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="31" t="s">
+      <c r="A34" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19" t="s">
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" s="31" t="s">
+      <c r="A35" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="66" t="s">
+      <c r="C35" s="38"/>
+      <c r="D35" s="38"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="G35" s="19" t="s">
+      <c r="G35" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
+      <c r="H35" s="38"/>
+      <c r="I35" s="38"/>
+      <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B36" s="31" t="s">
+      <c r="A36" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="64" t="s">
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="G36" s="19" t="s">
+      <c r="G36" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" s="31" t="s">
+      <c r="A37" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19" t="s">
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="H37" s="19"/>
-      <c r="I37" s="19"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="31" t="s">
+      <c r="A38" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19" t="s">
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="31" t="s">
+      <c r="A39" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="66" t="s">
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="G39" s="19" t="s">
+      <c r="G39" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="H39" s="21"/>
-      <c r="I39" s="19"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="31" t="s">
+      <c r="A40" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="54"/>
-      <c r="E40" s="51"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="51" t="s">
+      <c r="C40" s="38"/>
+      <c r="D40" s="42"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="H40" s="51"/>
-      <c r="I40" s="51"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="2"/>
     </row>
     <row r="41" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B41" s="31" t="s">
+      <c r="A41" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="51" t="s">
+      <c r="C41" s="38"/>
+      <c r="D41" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="E41" s="51" t="s">
+      <c r="E41" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="F41" s="51"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="51"/>
-      <c r="I41" s="51"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="2"/>
     </row>
     <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B42" s="31" t="s">
+      <c r="A42" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="51" t="s">
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="F42" s="51"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="51"/>
-      <c r="I42" s="51"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="2"/>
     </row>
     <row r="43" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B43" s="31" t="s">
+      <c r="A43" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="51"/>
-      <c r="E43" s="51" t="s">
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="F43" s="51"/>
-      <c r="G43" s="51"/>
-      <c r="H43" s="52"/>
-      <c r="I43" s="51"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="2"/>
     </row>
     <row r="44" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B44" s="31" t="s">
+      <c r="A44" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15" t="s">
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="F44" s="15"/>
-      <c r="G44" s="15"/>
-      <c r="H44" s="15" t="s">
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="I44" s="15" t="s">
+      <c r="I44" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B45" s="66" t="s">
+      <c r="A45" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
-      <c r="I45" s="15"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="2"/>
     </row>
     <row r="46" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B46" s="66" t="s">
+      <c r="A46" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
-      <c r="G46" s="15"/>
-      <c r="H46" s="15"/>
-      <c r="I46" s="15"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="36"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="2"/>
     </row>
     <row r="47" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B47" s="66" t="s">
+      <c r="A47" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="56" t="s">
+      <c r="C47" s="36"/>
+      <c r="D47" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="E47" s="15" t="s">
+      <c r="E47" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F47" s="15"/>
-      <c r="G47" s="15"/>
-      <c r="H47" s="15"/>
-      <c r="I47" s="15"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="2"/>
     </row>
     <row r="48" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B48" s="66" t="s">
+      <c r="A48" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15" t="s">
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="F48" s="15"/>
-      <c r="G48" s="15"/>
-      <c r="H48" s="15"/>
-      <c r="I48" s="15"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="36"/>
+      <c r="J48" s="2"/>
     </row>
     <row r="49" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B49" s="66" t="s">
+      <c r="A49" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15" t="s">
+      <c r="C49" s="36"/>
+      <c r="D49" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="E49" s="15" t="s">
+      <c r="E49" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F49" s="15"/>
-      <c r="G49" s="15"/>
-      <c r="H49" s="15"/>
-      <c r="I49" s="15"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
+      <c r="I49" s="36"/>
+      <c r="J49" s="2"/>
     </row>
     <row r="50" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B50" s="66" t="s">
+      <c r="A50" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15" t="s">
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
-      <c r="H50" s="15"/>
-      <c r="I50" s="15"/>
+      <c r="F50" s="36"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="36"/>
+      <c r="J50" s="2"/>
     </row>
     <row r="51" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B51" s="66" t="s">
+      <c r="A51" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="15" t="s">
+      <c r="C51" s="36"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
-      <c r="H51" s="15"/>
-      <c r="I51" s="15"/>
+      <c r="F51" s="36"/>
+      <c r="G51" s="36"/>
+      <c r="H51" s="36"/>
+      <c r="I51" s="36"/>
+      <c r="J51" s="2"/>
     </row>
     <row r="52" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B52" s="66" t="s">
+      <c r="A52" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15"/>
-      <c r="E52" s="15" t="s">
+      <c r="C52" s="36"/>
+      <c r="D52" s="36"/>
+      <c r="E52" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="F52" s="15"/>
-      <c r="G52" s="15"/>
-      <c r="H52" s="15" t="s">
+      <c r="F52" s="36"/>
+      <c r="G52" s="36"/>
+      <c r="H52" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="I52" s="15" t="s">
+      <c r="I52" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J52">
+      <c r="J52" s="2">
         <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B53" s="67" t="s">
+      <c r="A53" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B53" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C53" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="15"/>
-      <c r="E53" s="15"/>
-      <c r="F53" s="15"/>
-      <c r="G53" s="15"/>
-      <c r="H53" s="15"/>
-      <c r="I53" s="15"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="36"/>
+      <c r="F53" s="36"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="36"/>
+      <c r="I53" s="36"/>
+      <c r="J53" s="2"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B54" s="67" t="s">
+      <c r="A54" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B54" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C54" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D54" s="56"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="36"/>
+      <c r="F54" s="36"/>
+      <c r="G54" s="36"/>
+      <c r="H54" s="36"/>
+      <c r="I54" s="36"/>
+      <c r="J54" s="2"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B55" s="67" t="s">
+      <c r="A55" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="C55" s="14" t="s">
+      <c r="C55" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14" t="s">
+      <c r="D55" s="36"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="36"/>
+      <c r="G55" s="36"/>
+      <c r="H55" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="I55" s="14" t="s">
+      <c r="I55" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="J55">
+      <c r="J55" s="2">
         <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B56" s="14" t="s">
+      <c r="A56" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B56" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="C56" s="14" t="s">
+      <c r="C56" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
+      <c r="D56" s="36"/>
+      <c r="E56" s="36"/>
+      <c r="F56" s="36"/>
+      <c r="G56" s="36"/>
+      <c r="H56" s="36"/>
+      <c r="I56" s="36"/>
+      <c r="J56" s="2"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14" t="s">
+      <c r="A57" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="36"/>
       <c r="F57" s="22"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
+      <c r="G57" s="36"/>
+      <c r="H57" s="36"/>
+      <c r="I57" s="36"/>
+      <c r="J57" s="2"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14" t="s">
+      <c r="A58" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B58" s="36"/>
+      <c r="C58" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
+      <c r="D58" s="36"/>
+      <c r="E58" s="36"/>
       <c r="F58" s="22"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14" t="s">
+      <c r="G58" s="36"/>
+      <c r="H58" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="I58" s="14" t="s">
+      <c r="I58" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J58">
+      <c r="J58" s="2">
         <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14" t="s">
+      <c r="A59" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D59" s="56"/>
-      <c r="E59" s="14"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="36"/>
       <c r="F59" s="22"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14" t="s">
+      <c r="G59" s="36"/>
+      <c r="H59" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="I59" s="14" t="s">
+      <c r="I59" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J59">
+      <c r="J59" s="2">
         <v>16</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B60" s="15" t="s">
+      <c r="A60" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B60" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C60" s="15" t="s">
+      <c r="C60" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D60" s="15"/>
-      <c r="E60" s="15"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="15" t="s">
+      <c r="D60" s="36"/>
+      <c r="E60" s="36"/>
+      <c r="F60" s="36"/>
+      <c r="G60" s="36"/>
+      <c r="H60" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="I60" s="15" t="s">
+      <c r="I60" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J60">
+      <c r="J60" s="2">
         <v>17</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B61" s="15" t="s">
+      <c r="A61" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C61" s="15" t="s">
+      <c r="C61" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D61" s="15"/>
-      <c r="E61" s="15"/>
-      <c r="F61" s="15"/>
-      <c r="G61" s="15"/>
-      <c r="H61" s="15" t="s">
+      <c r="D61" s="36"/>
+      <c r="E61" s="36"/>
+      <c r="F61" s="36"/>
+      <c r="G61" s="36"/>
+      <c r="H61" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="I61" s="15" t="s">
+      <c r="I61" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="J61">
+      <c r="J61" s="2">
         <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="43"/>
-      <c r="B62" s="15" t="s">
+      <c r="A62" s="25"/>
+      <c r="B62" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C62" s="15" t="s">
+      <c r="C62" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D62" s="15"/>
-      <c r="E62" s="15"/>
-      <c r="F62" s="15"/>
-      <c r="G62" s="15"/>
-      <c r="H62" s="15" t="s">
+      <c r="D62" s="36"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="36"/>
+      <c r="G62" s="36"/>
+      <c r="H62" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="I62" s="15" t="s">
+      <c r="I62" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J62">
+      <c r="J62" s="2">
         <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="43"/>
-      <c r="B63" s="15" t="s">
+      <c r="A63" s="25"/>
+      <c r="B63" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C63" s="15" t="s">
+      <c r="C63" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D63" s="15"/>
-      <c r="E63" s="15"/>
-      <c r="F63" s="15"/>
-      <c r="G63" s="15"/>
-      <c r="H63" s="24" t="s">
+      <c r="D63" s="36"/>
+      <c r="E63" s="36"/>
+      <c r="F63" s="36"/>
+      <c r="G63" s="36"/>
+      <c r="H63" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="I63" s="15" t="s">
+      <c r="I63" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="J63">
+      <c r="J63" s="2">
         <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B64" s="24" t="s">
+      <c r="A64" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B64" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C64" s="24" t="s">
+      <c r="C64" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D64" s="24"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="24"/>
-      <c r="G64" s="24"/>
-      <c r="H64" s="68" t="s">
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="I64" s="24" t="s">
+      <c r="I64" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="J64">
+      <c r="J64" s="2">
         <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" s="43" t="s">
-        <v>35</v>
-      </c>
-      <c r="B65" s="24" t="s">
+      <c r="A65" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B65" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C65" s="24" t="s">
+      <c r="C65" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D65" s="24"/>
-      <c r="E65" s="24"/>
-      <c r="F65" s="24"/>
-      <c r="G65" s="24"/>
-      <c r="H65" s="24" t="s">
+      <c r="D65" s="16"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="I65" s="24" t="s">
+      <c r="I65" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J65">
+      <c r="J65" s="2">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
guion 1 grado 9 definitivos
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/EsqueletoGuion_CS_09_01_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion01/EsqueletoGuion_CS_09_01_CO.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MCMarquez\Desktop\Versiones\CienciasSociales\fuentes\contenidos\grado09\guion01\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9255" tabRatio="729" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9255" tabRatio="729" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -18,7 +13,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +31,7 @@
     <author>MCMarquez</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0">
+    <comment ref="B6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="91">
   <si>
     <t>FICHA</t>
   </si>
@@ -361,6 +356,9 @@
   </si>
   <si>
     <t>Refuerza tu aprendizaje:  El colonialismo y sus causas</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La dominación, organización y explotación de las colonias</t>
   </si>
 </sst>
 </file>
@@ -1821,7 +1819,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2767,8 +2765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="76" zoomScaleNormal="76" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="I73" sqref="I73"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="57" zoomScaleNormal="57" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2904,22 +2902,18 @@
       <c r="B6" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="76"/>
-      <c r="E6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="76" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>24</v>
+      </c>
       <c r="F6" s="41"/>
       <c r="G6" s="41"/>
-      <c r="H6" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="36">
-        <v>3</v>
-      </c>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="36"/>
     </row>
     <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
@@ -2928,66 +2922,64 @@
       <c r="B7" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="76" t="s">
+      <c r="C7" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="39" t="s">
         <v>75</v>
       </c>
       <c r="E7" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="52" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="36"/>
-    </row>
-    <row r="8" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="J8" s="36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" s="52" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="51"/>
+    </row>
+    <row r="9" spans="1:10" s="52" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="48" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="50" t="s">
-        <v>24</v>
+      <c r="C9" s="49" t="s">
+        <v>34</v>
       </c>
       <c r="D9" s="49"/>
       <c r="E9" s="49"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="50"/>
-      <c r="H9" s="70"/>
-      <c r="I9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
       <c r="J9" s="51"/>
     </row>
-    <row r="10" spans="1:10" s="52" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="52" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48" t="s">
         <v>30</v>
       </c>
@@ -2995,12 +2987,12 @@
         <v>38</v>
       </c>
       <c r="C10" s="49" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="49"/>
+        <v>39</v>
+      </c>
+      <c r="D10" s="71"/>
       <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
       <c r="H10" s="48"/>
       <c r="I10" s="48"/>
       <c r="J10" s="51"/>
@@ -3012,11 +3004,13 @@
       <c r="B11" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="71"/>
-      <c r="E11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="71" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="49" t="s">
+        <v>24</v>
+      </c>
       <c r="F11" s="50"/>
       <c r="G11" s="50"/>
       <c r="H11" s="48"/>
@@ -3030,44 +3024,42 @@
       <c r="B12" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="71" t="s">
+      <c r="C12" s="50"/>
+      <c r="D12" s="49" t="s">
         <v>75</v>
       </c>
       <c r="E12" s="49" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F12" s="50"/>
       <c r="G12" s="50"/>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="51"/>
-    </row>
-    <row r="13" spans="1:10" s="52" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="E13" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" s="48" t="s">
+      <c r="H12" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="51">
+      <c r="J12" s="51">
         <v>5</v>
       </c>
+    </row>
+    <row r="13" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="55"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="53" t="s">
@@ -3076,11 +3068,13 @@
       <c r="B14" s="54" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="53"/>
+      <c r="D14" s="77" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
       <c r="F14" s="56"/>
       <c r="G14" s="56"/>
       <c r="H14" s="53"/>
@@ -3099,7 +3093,7 @@
         <v>42</v>
       </c>
       <c r="E15" s="56" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F15" s="56"/>
       <c r="G15" s="56"/>
@@ -3119,12 +3113,16 @@
         <v>42</v>
       </c>
       <c r="E16" s="56" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F16" s="56"/>
       <c r="G16" s="56"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
+      <c r="H16" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="53" t="s">
+        <v>20</v>
+      </c>
       <c r="J16" s="57"/>
     </row>
     <row r="17" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CS0901: Ajustes de Esqueleto, Solicitud gráfica y nombres
Carga de documento de seguimiento de producción digital.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion01/EsqueletoGuion_CS_09_01_CO.xlsx
+++ b/fuentes/contenidos/grado09/guion01/EsqueletoGuion_CS_09_01_CO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasSociales\fuentes\contenidos\grado09\guion01\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9255" tabRatio="729" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18765" windowHeight="9258" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +36,7 @@
     <author>MCMarquez</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -56,37 +61,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>MCMarquez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Ciencias Sociales
-</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="85">
   <si>
     <t>FICHA</t>
   </si>
@@ -184,9 +164,6 @@
     <t>El colonialismo y sus causas</t>
   </si>
   <si>
-    <t>La última fase del colonialismo: el imperialismo</t>
-  </si>
-  <si>
     <t>CS_10_06</t>
   </si>
   <si>
@@ -292,9 +269,6 @@
     <t>Las consecuencias de la Guerra</t>
   </si>
   <si>
-    <t>Cronología: el imperialismo y la Primera Guerra Mundial</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: Las consecuencias de la guerra</t>
   </si>
   <si>
@@ -307,9 +281,6 @@
     <t>Identifica las causas y evolución de la Primera Guerra Mundial</t>
   </si>
   <si>
-    <t>Identifica las causas y evolución de la primera Guerra mundial</t>
-  </si>
-  <si>
     <t>Proyecto: Análisis del colonialismo español</t>
   </si>
   <si>
@@ -325,9 +296,6 @@
     <t>El imperialismo y la Primera Guerra</t>
   </si>
   <si>
-    <t>Ciencias sociales</t>
-  </si>
-  <si>
     <t>CS_09_01_CO</t>
   </si>
   <si>
@@ -343,22 +311,16 @@
     <t>Refuerza tu aprendizaje: El colonialismo y sus causas</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje: Las consencuencias El imperialismo</t>
-  </si>
-  <si>
     <t>Cronología: El imperialismo y la Primera Guerra Mundial</t>
   </si>
   <si>
-    <t>Competencias: Comentario de un mapa de la Primera Guerra Mundial</t>
-  </si>
-  <si>
     <t>La última fase del colonialismo: El imperialismo</t>
   </si>
   <si>
-    <t>Refuerza tu aprendizaje:  El colonialismo y sus causas</t>
-  </si>
-  <si>
-    <t>Refuerza tu aprendizaje: La dominación, organización y explotación de las colonias</t>
+    <t>Ciencias Sociales</t>
+  </si>
+  <si>
+    <t>4º ESO</t>
   </si>
 </sst>
 </file>
@@ -1819,7 +1781,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1829,49 +1791,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="104.265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1879,12 +1839,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1904,22 +1864,22 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.73046875" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1939,7 +1899,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="17" t="s">
         <v>27</v>
       </c>
@@ -1950,10 +1910,10 @@
         <v>30</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="17">
         <v>1</v>
@@ -1965,21 +1925,21 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="17" t="s">
+    <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>33</v>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
       </c>
       <c r="F3" s="17">
         <v>2</v>
@@ -1991,7 +1951,7 @@
       <c r="K3"/>
       <c r="L3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="17" t="s">
         <v>27</v>
       </c>
@@ -2002,16 +1962,16 @@
         <v>30</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F4" s="17">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="17" t="s">
         <v>27</v>
       </c>
@@ -2022,16 +1982,16 @@
         <v>30</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F5" s="18">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="17" t="s">
         <v>27</v>
       </c>
@@ -2042,16 +2002,16 @@
         <v>30</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" s="17">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="17" t="s">
         <v>27</v>
       </c>
@@ -2062,16 +2022,16 @@
         <v>30</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" s="17">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="17" t="s">
         <v>27</v>
       </c>
@@ -2082,16 +2042,16 @@
         <v>30</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="17">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="17" t="s">
         <v>27</v>
       </c>
@@ -2102,16 +2062,16 @@
         <v>30</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="17">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="17" t="s">
         <v>27</v>
       </c>
@@ -2122,17 +2082,17 @@
         <v>30</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F10" s="17">
         <v>11</v>
       </c>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="17" t="s">
         <v>27</v>
       </c>
@@ -2143,17 +2103,17 @@
         <v>30</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="17">
         <v>12</v>
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="17" t="s">
         <v>27</v>
       </c>
@@ -2164,17 +2124,17 @@
         <v>30</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="17">
         <v>13</v>
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="17" t="s">
         <v>27</v>
       </c>
@@ -2185,17 +2145,17 @@
         <v>30</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="17">
         <v>14</v>
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="17" t="s">
         <v>27</v>
       </c>
@@ -2206,16 +2166,16 @@
         <v>30</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="17">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="17" t="s">
         <v>27</v>
       </c>
@@ -2226,16 +2186,16 @@
         <v>30</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" s="17">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="17" t="s">
         <v>27</v>
       </c>
@@ -2246,16 +2206,16 @@
         <v>30</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F16" s="17">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="17" t="s">
         <v>27</v>
       </c>
@@ -2266,16 +2226,16 @@
         <v>30</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" s="17">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="17" t="s">
         <v>27</v>
       </c>
@@ -2286,10 +2246,10 @@
         <v>30</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" s="17">
         <v>20</v>
@@ -2311,16 +2271,16 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="66.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="66.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -2331,9 +2291,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>21</v>
@@ -2342,9 +2302,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>21</v>
@@ -2353,9 +2313,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>21</v>
@@ -2364,7 +2324,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="15" t="s">
         <v>22</v>
       </c>
@@ -2375,7 +2335,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="15" t="s">
         <v>23</v>
       </c>
@@ -2408,17 +2368,17 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C19" sqref="B19:C19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -2429,227 +2389,227 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="14">
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="14">
         <v>2</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="14">
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="14">
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="14">
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="14">
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="14">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="14">
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="14">
         <v>9</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="14">
         <v>10</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="14">
         <v>11</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="14">
         <v>12</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="14">
         <v>13</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="14">
         <v>14</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="14">
         <v>15</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="14">
         <v>16</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="14">
         <v>17</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="14">
         <v>18</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="14">
         <v>19</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="14">
         <v>20</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="14">
         <v>21</v>
       </c>
@@ -2660,7 +2620,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="14">
         <v>22</v>
       </c>
@@ -2671,77 +2631,77 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="25"/>
       <c r="B24" s="25"/>
       <c r="C24" s="23"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="22"/>
       <c r="B25" s="22"/>
       <c r="C25" s="23"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="22"/>
       <c r="B26" s="22"/>
       <c r="C26" s="23"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="22"/>
       <c r="B27" s="22"/>
       <c r="C27" s="23"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="22"/>
       <c r="B28" s="22"/>
       <c r="C28" s="23"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="22"/>
       <c r="B29" s="22"/>
       <c r="C29" s="23"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="22"/>
       <c r="B30" s="22"/>
       <c r="C30" s="23"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="22"/>
       <c r="B31" s="22"/>
       <c r="C31" s="23"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="22"/>
       <c r="B32" s="22"/>
       <c r="C32" s="23"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="22"/>
       <c r="B33" s="22"/>
       <c r="C33" s="23"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="22"/>
       <c r="B34" s="22"/>
       <c r="C34" s="23"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="22"/>
       <c r="B35" s="22"/>
       <c r="C35" s="23"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="23"/>
       <c r="B36" s="23"/>
       <c r="C36" s="24"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="23"/>
       <c r="B37" s="23"/>
       <c r="C37" s="24"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="23"/>
       <c r="B38" s="23"/>
       <c r="C38" s="24"/>
@@ -2765,23 +2725,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="57" zoomScaleNormal="57" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView zoomScale="57" zoomScaleNormal="57" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="51.85546875" style="21" customWidth="1"/>
-    <col min="2" max="2" width="58.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
-    <col min="5" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.06640625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="42.9296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.9296875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.86328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="36.9296875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="20" t="s">
         <v>6</v>
       </c>
@@ -2811,7 +2773,7 @@
       </c>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="40" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A2" s="37" t="s">
         <v>30</v>
       </c>
@@ -2829,7 +2791,7 @@
       <c r="I2" s="37"/>
       <c r="J2" s="36"/>
     </row>
-    <row r="3" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="40" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A3" s="37" t="s">
         <v>30</v>
       </c>
@@ -2844,7 +2806,7 @@
       <c r="F3" s="39"/>
       <c r="G3" s="39"/>
       <c r="H3" s="37" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="I3" s="37" t="s">
         <v>20</v>
@@ -2853,7 +2815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="40" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A4" s="37" t="s">
         <v>30</v>
       </c>
@@ -2861,7 +2823,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="39"/>
       <c r="E4" s="39"/>
@@ -2871,7 +2833,7 @@
       <c r="I4" s="37"/>
       <c r="J4" s="36"/>
     </row>
-    <row r="5" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="40" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A5" s="37" t="s">
         <v>30</v>
       </c>
@@ -2879,14 +2841,14 @@
         <v>31</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5" s="39"/>
       <c r="E5" s="39"/>
       <c r="F5" s="39"/>
       <c r="G5" s="39"/>
       <c r="H5" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I5" s="37" t="s">
         <v>20</v>
@@ -2895,7 +2857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="40" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A6" s="37" t="s">
         <v>30</v>
       </c>
@@ -2904,7 +2866,7 @@
       </c>
       <c r="C6" s="39"/>
       <c r="D6" s="76" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E6" s="39" t="s">
         <v>24</v>
@@ -2915,7 +2877,7 @@
       <c r="I6" s="42"/>
       <c r="J6" s="36"/>
     </row>
-    <row r="7" spans="1:10" s="40" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="40" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A7" s="37" t="s">
         <v>30</v>
       </c>
@@ -2923,18 +2885,18 @@
         <v>31</v>
       </c>
       <c r="C7" s="39" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E7" s="39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="39"/>
       <c r="G7" s="39"/>
       <c r="H7" s="37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I7" s="37" t="s">
         <v>20</v>
@@ -2943,12 +2905,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="52" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="52" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A8" s="48" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="50" t="s">
         <v>24</v>
@@ -2961,15 +2923,15 @@
       <c r="I8" s="49"/>
       <c r="J8" s="51"/>
     </row>
-    <row r="9" spans="1:10" s="52" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="52" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="48" t="s">
         <v>30</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="49"/>
       <c r="E9" s="49"/>
@@ -2979,15 +2941,15 @@
       <c r="I9" s="48"/>
       <c r="J9" s="51"/>
     </row>
-    <row r="10" spans="1:10" s="52" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="52" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A10" s="48" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="49" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" s="49" t="s">
-        <v>39</v>
       </c>
       <c r="D10" s="71"/>
       <c r="E10" s="49"/>
@@ -2997,16 +2959,16 @@
       <c r="I10" s="48"/>
       <c r="J10" s="51"/>
     </row>
-    <row r="11" spans="1:10" s="52" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="52" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A11" s="48" t="s">
         <v>30</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="49"/>
       <c r="D11" s="71" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E11" s="49" t="s">
         <v>24</v>
@@ -3017,24 +2979,24 @@
       <c r="I11" s="48"/>
       <c r="J11" s="51"/>
     </row>
-    <row r="12" spans="1:10" s="52" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="52" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="48" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="50"/>
       <c r="D12" s="49" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E12" s="49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F12" s="50"/>
       <c r="G12" s="50"/>
       <c r="H12" s="48" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="I12" s="48" t="s">
         <v>20</v>
@@ -3043,12 +3005,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A13" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="53" t="s">
         <v>24</v>
@@ -3061,16 +3023,16 @@
       <c r="I13" s="53"/>
       <c r="J13" s="57"/>
     </row>
-    <row r="14" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="58" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A14" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="53"/>
       <c r="D14" s="77" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E14" s="56" t="s">
         <v>24</v>
@@ -3081,19 +3043,19 @@
       <c r="I14" s="53"/>
       <c r="J14" s="57"/>
     </row>
-    <row r="15" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="58" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A15" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="53"/>
       <c r="D15" s="77" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="56" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="56"/>
       <c r="G15" s="56"/>
@@ -3101,16 +3063,16 @@
       <c r="I15" s="53"/>
       <c r="J15" s="57"/>
     </row>
-    <row r="16" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="58" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A16" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B16" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="53"/>
       <c r="D16" s="77" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E16" s="56" t="s">
         <v>25</v>
@@ -3118,23 +3080,23 @@
       <c r="F16" s="56"/>
       <c r="G16" s="56"/>
       <c r="H16" s="53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I16" s="53" t="s">
         <v>20</v>
       </c>
       <c r="J16" s="57"/>
     </row>
-    <row r="17" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A17" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="53"/>
       <c r="D17" s="55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E17" s="56" t="s">
         <v>24</v>
@@ -3145,16 +3107,16 @@
       <c r="I17" s="53"/>
       <c r="J17" s="57"/>
     </row>
-    <row r="18" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="58" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A18" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="53"/>
       <c r="D18" s="55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" s="56" t="s">
         <v>25</v>
@@ -3162,7 +3124,7 @@
       <c r="F18" s="56"/>
       <c r="G18" s="56"/>
       <c r="H18" s="72" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I18" s="53" t="s">
         <v>20</v>
@@ -3171,16 +3133,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="58" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A19" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="60"/>
       <c r="D19" s="60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" s="60" t="s">
         <v>24</v>
@@ -3191,19 +3153,19 @@
       <c r="I19" s="60"/>
       <c r="J19" s="57"/>
     </row>
-    <row r="20" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A20" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="60"/>
       <c r="D20" s="60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="60" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F20" s="60"/>
       <c r="G20" s="60"/>
@@ -3211,16 +3173,16 @@
       <c r="I20" s="60"/>
       <c r="J20" s="57"/>
     </row>
-    <row r="21" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A21" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="60"/>
       <c r="D21" s="60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" s="60" t="s">
         <v>24</v>
@@ -3231,24 +3193,24 @@
       <c r="I21" s="60"/>
       <c r="J21" s="57"/>
     </row>
-    <row r="22" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A22" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B22" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="60"/>
       <c r="D22" s="60" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E22" s="60" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" s="60"/>
       <c r="G22" s="60"/>
       <c r="H22" s="60" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I22" s="60" t="s">
         <v>21</v>
@@ -3257,16 +3219,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A23" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" s="60"/>
       <c r="D23" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="60" t="s">
         <v>24</v>
@@ -3277,19 +3239,19 @@
       <c r="I23" s="60"/>
       <c r="J23" s="57"/>
     </row>
-    <row r="24" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A24" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B24" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" s="60"/>
       <c r="D24" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="60" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F24" s="60"/>
       <c r="G24" s="60"/>
@@ -3297,16 +3259,16 @@
       <c r="I24" s="60"/>
       <c r="J24" s="57"/>
     </row>
-    <row r="25" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A25" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B25" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="60"/>
       <c r="D25" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E25" s="60" t="s">
         <v>25</v>
@@ -3314,7 +3276,7 @@
       <c r="F25" s="60"/>
       <c r="G25" s="60"/>
       <c r="H25" s="60" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I25" s="60" t="s">
         <v>20</v>
@@ -3323,16 +3285,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A26" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26" s="60"/>
       <c r="D26" s="60" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E26" s="60" t="s">
         <v>24</v>
@@ -3343,24 +3305,24 @@
       <c r="I26" s="60"/>
       <c r="J26" s="57"/>
     </row>
-    <row r="27" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A27" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27" s="60"/>
       <c r="D27" s="61" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E27" s="60" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F27" s="60"/>
       <c r="G27" s="60"/>
       <c r="H27" s="60" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I27" s="60" t="s">
         <v>20</v>
@@ -3369,12 +3331,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A28" s="19" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" s="30" t="s">
         <v>24</v>
@@ -3387,15 +3349,15 @@
       <c r="I28" s="30"/>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A29" s="19" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" s="69"/>
       <c r="E29" s="30"/>
@@ -3405,15 +3367,15 @@
       <c r="I29" s="30"/>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A30" s="19" t="s">
         <v>30</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D30" s="31"/>
       <c r="E30" s="30"/>
@@ -3423,16 +3385,16 @@
       <c r="I30" s="30"/>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A31" s="19" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C31" s="30"/>
       <c r="D31" s="30" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E31" s="30" t="s">
         <v>24</v>
@@ -3443,24 +3405,24 @@
       <c r="I31" s="30"/>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A32" s="19" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C32" s="37"/>
       <c r="D32" s="30" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F32" s="30"/>
       <c r="G32" s="30"/>
       <c r="H32" s="30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I32" s="30" t="s">
         <v>21</v>
@@ -3469,12 +3431,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" s="66" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A33" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B33" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="64" t="s">
         <v>24</v>
@@ -3487,12 +3449,12 @@
       <c r="I33" s="64"/>
       <c r="J33" s="65"/>
     </row>
-    <row r="34" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" s="66" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A34" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B34" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" s="64" t="s">
         <v>25</v>
@@ -3502,7 +3464,7 @@
       <c r="F34" s="64"/>
       <c r="G34" s="64"/>
       <c r="H34" s="64" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I34" s="64" t="s">
         <v>20</v>
@@ -3511,16 +3473,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" s="66" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A35" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C35" s="64"/>
       <c r="D35" s="67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E35" s="68" t="s">
         <v>24</v>
@@ -3531,19 +3493,19 @@
       <c r="I35" s="64"/>
       <c r="J35" s="65"/>
     </row>
-    <row r="36" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" s="66" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A36" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C36" s="64"/>
       <c r="D36" s="67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E36" s="64" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F36" s="64"/>
       <c r="G36" s="64"/>
@@ -3551,20 +3513,20 @@
       <c r="I36" s="64"/>
       <c r="J36" s="65"/>
     </row>
-    <row r="37" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" s="66" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A37" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C37" s="64"/>
       <c r="D37" s="67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E37" s="64"/>
       <c r="F37" s="64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G37" s="64" t="s">
         <v>24</v>
@@ -3573,42 +3535,42 @@
       <c r="I37" s="64"/>
       <c r="J37" s="65"/>
     </row>
-    <row r="38" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" s="66" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A38" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B38" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C38" s="64"/>
       <c r="D38" s="67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E38" s="64"/>
       <c r="F38" s="64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G38" s="64" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H38" s="64"/>
       <c r="I38" s="64"/>
       <c r="J38" s="65"/>
     </row>
-    <row r="39" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" s="66" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A39" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B39" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C39" s="64"/>
       <c r="D39" s="67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E39" s="64"/>
       <c r="F39" s="74" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G39" s="64" t="s">
         <v>24</v>
@@ -3617,20 +3579,20 @@
       <c r="I39" s="64"/>
       <c r="J39" s="65"/>
     </row>
-    <row r="40" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" s="66" customFormat="1" ht="15.85" x14ac:dyDescent="0.45">
       <c r="A40" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B40" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C40" s="64"/>
       <c r="D40" s="67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E40" s="64"/>
       <c r="F40" s="75" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G40" s="64" t="s">
         <v>24</v>
@@ -3639,42 +3601,42 @@
       <c r="I40" s="64"/>
       <c r="J40" s="65"/>
     </row>
-    <row r="41" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" s="66" customFormat="1" ht="15.85" x14ac:dyDescent="0.45">
       <c r="A41" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B41" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C41" s="64"/>
       <c r="D41" s="67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E41" s="64"/>
       <c r="F41" s="75" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G41" s="64" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H41" s="64"/>
       <c r="I41" s="64"/>
       <c r="J41" s="65"/>
     </row>
-    <row r="42" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" s="66" customFormat="1" ht="15.85" x14ac:dyDescent="0.45">
       <c r="A42" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B42" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C42" s="64"/>
       <c r="D42" s="67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E42" s="64"/>
       <c r="F42" s="75" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G42" s="64" t="s">
         <v>24</v>
@@ -3683,20 +3645,20 @@
       <c r="I42" s="64"/>
       <c r="J42" s="65"/>
     </row>
-    <row r="43" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" s="66" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A43" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B43" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C43" s="64"/>
       <c r="D43" s="67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E43" s="64"/>
       <c r="F43" s="74" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G43" s="64" t="s">
         <v>24</v>
@@ -3705,38 +3667,38 @@
       <c r="I43" s="64"/>
       <c r="J43" s="65"/>
     </row>
-    <row r="44" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" s="66" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A44" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B44" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C44" s="64"/>
       <c r="D44" s="67" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E44" s="64"/>
       <c r="F44" s="74" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G44" s="64" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H44" s="64"/>
       <c r="I44" s="64"/>
       <c r="J44" s="65"/>
     </row>
-    <row r="45" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" s="66" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A45" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B45" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C45" s="64"/>
       <c r="D45" s="64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E45" s="64" t="s">
         <v>24</v>
@@ -3747,19 +3709,19 @@
       <c r="I45" s="64"/>
       <c r="J45" s="65"/>
     </row>
-    <row r="46" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" s="66" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A46" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B46" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C46" s="64"/>
       <c r="D46" s="64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E46" s="64" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F46" s="64"/>
       <c r="G46" s="64"/>
@@ -3767,16 +3729,16 @@
       <c r="I46" s="64"/>
       <c r="J46" s="65"/>
     </row>
-    <row r="47" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" s="66" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A47" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B47" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C47" s="64"/>
       <c r="D47" s="64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E47" s="64" t="s">
         <v>24</v>
@@ -3787,16 +3749,16 @@
       <c r="I47" s="64"/>
       <c r="J47" s="65"/>
     </row>
-    <row r="48" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" s="66" customFormat="1" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A48" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B48" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C48" s="64"/>
       <c r="D48" s="62" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E48" s="64" t="s">
         <v>24</v>
@@ -3807,24 +3769,24 @@
       <c r="I48" s="64"/>
       <c r="J48" s="65"/>
     </row>
-    <row r="49" spans="1:10" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" s="66" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A49" s="62" t="s">
         <v>30</v>
       </c>
       <c r="B49" s="63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C49" s="62"/>
       <c r="D49" s="62" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E49" s="62" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F49" s="62"/>
       <c r="G49" s="62"/>
       <c r="H49" s="62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I49" s="62" t="s">
         <v>20</v>
@@ -3833,15 +3795,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A50" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B50" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="53" t="s">
         <v>61</v>
-      </c>
-      <c r="C50" s="53" t="s">
-        <v>62</v>
       </c>
       <c r="D50" s="53"/>
       <c r="E50" s="53"/>
@@ -3851,16 +3813,16 @@
       <c r="I50" s="53"/>
       <c r="J50" s="57"/>
     </row>
-    <row r="51" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A51" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B51" s="59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51" s="53"/>
       <c r="D51" s="53" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E51" s="53" t="s">
         <v>24</v>
@@ -3871,19 +3833,19 @@
       <c r="I51" s="53"/>
       <c r="J51" s="57"/>
     </row>
-    <row r="52" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A52" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B52" s="59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C52" s="53"/>
       <c r="D52" s="53" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E52" s="53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F52" s="53"/>
       <c r="G52" s="53"/>
@@ -3891,16 +3853,16 @@
       <c r="I52" s="53"/>
       <c r="J52" s="57"/>
     </row>
-    <row r="53" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A53" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B53" s="59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C53" s="53"/>
       <c r="D53" s="53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E53" s="53" t="s">
         <v>24</v>
@@ -3911,19 +3873,19 @@
       <c r="I53" s="53"/>
       <c r="J53" s="57"/>
     </row>
-    <row r="54" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A54" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B54" s="59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C54" s="53"/>
       <c r="D54" s="53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E54" s="53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F54" s="53"/>
       <c r="G54" s="53"/>
@@ -3931,16 +3893,16 @@
       <c r="I54" s="53"/>
       <c r="J54" s="57"/>
     </row>
-    <row r="55" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A55" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B55" s="59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C55" s="53"/>
       <c r="D55" s="53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E55" s="53" t="s">
         <v>24</v>
@@ -3951,19 +3913,19 @@
       <c r="I55" s="53"/>
       <c r="J55" s="57"/>
     </row>
-    <row r="56" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A56" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B56" s="59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C56" s="53"/>
       <c r="D56" s="53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E56" s="53" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F56" s="53"/>
       <c r="G56" s="53"/>
@@ -3971,16 +3933,16 @@
       <c r="I56" s="53"/>
       <c r="J56" s="57"/>
     </row>
-    <row r="57" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A57" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B57" s="59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C57" s="53"/>
       <c r="D57" s="53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E57" s="53" t="s">
         <v>24</v>
@@ -3991,16 +3953,16 @@
       <c r="I57" s="53"/>
       <c r="J57" s="57"/>
     </row>
-    <row r="58" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A58" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B58" s="59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C58" s="53"/>
       <c r="D58" s="53" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E58" s="53" t="s">
         <v>24</v>
@@ -4011,24 +3973,24 @@
       <c r="I58" s="53"/>
       <c r="J58" s="57"/>
     </row>
-    <row r="59" spans="1:10" s="58" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" s="58" customFormat="1" ht="15.45" x14ac:dyDescent="0.45">
       <c r="A59" s="53" t="s">
         <v>30</v>
       </c>
       <c r="B59" s="59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C59" s="53"/>
       <c r="D59" s="53" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E59" s="55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F59" s="53"/>
       <c r="G59" s="53"/>
       <c r="H59" s="53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I59" s="53" t="s">
         <v>20</v>
@@ -4037,12 +3999,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A60" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60" s="16" t="s">
         <v>24</v>
@@ -4055,15 +4017,15 @@
       <c r="I60" s="16"/>
       <c r="J60" s="28"/>
     </row>
-    <row r="61" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A61" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C61" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D61" s="16"/>
       <c r="E61" s="16"/>
@@ -4073,16 +4035,16 @@
       <c r="I61" s="16"/>
       <c r="J61" s="28"/>
     </row>
-    <row r="62" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A62" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C62" s="16"/>
       <c r="D62" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E62" s="16" t="s">
         <v>24</v>
@@ -4093,24 +4055,24 @@
       <c r="I62" s="16"/>
       <c r="J62" s="28"/>
     </row>
-    <row r="63" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" s="43" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A63" s="16" t="s">
         <v>30</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C63" s="16"/>
       <c r="D63" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E63" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F63" s="16"/>
       <c r="G63" s="16"/>
       <c r="H63" s="16" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I63" s="16" t="s">
         <v>28</v>
@@ -4119,12 +4081,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A64" s="44" t="s">
         <v>30</v>
       </c>
       <c r="B64" s="44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C64" s="44" t="s">
         <v>24</v>
@@ -4137,12 +4099,12 @@
       <c r="I64" s="44"/>
       <c r="J64" s="46"/>
     </row>
-    <row r="65" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A65" s="44" t="s">
         <v>30</v>
       </c>
       <c r="B65" s="44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C65" s="44" t="s">
         <v>25</v>
@@ -4152,7 +4114,7 @@
       <c r="F65" s="45"/>
       <c r="G65" s="44"/>
       <c r="H65" s="44" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="I65" s="44" t="s">
         <v>20</v>
@@ -4161,16 +4123,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A66" s="44" t="s">
         <v>30</v>
       </c>
       <c r="B66" s="44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C66" s="44"/>
       <c r="D66" s="44" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E66" s="44" t="s">
         <v>24</v>
@@ -4181,24 +4143,24 @@
       <c r="I66" s="44"/>
       <c r="J66" s="46"/>
     </row>
-    <row r="67" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A67" s="44" t="s">
         <v>30</v>
       </c>
       <c r="B67" s="44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C67" s="44"/>
       <c r="D67" s="44" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E67" s="44" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F67" s="45"/>
       <c r="G67" s="44"/>
       <c r="H67" s="44" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I67" s="44" t="s">
         <v>20</v>
@@ -4207,7 +4169,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" s="47" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A68" s="44" t="s">
         <v>30</v>
       </c>
@@ -4225,7 +4187,7 @@
       <c r="I68" s="44"/>
       <c r="J68" s="46"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" s="19" t="s">
         <v>30</v>
       </c>
@@ -4233,14 +4195,14 @@
         <v>29</v>
       </c>
       <c r="C69" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D69" s="29"/>
       <c r="E69" s="29"/>
       <c r="F69" s="29"/>
       <c r="G69" s="29"/>
       <c r="H69" s="29" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="I69" s="29" t="s">
         <v>20</v>
@@ -4249,7 +4211,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" s="19" t="s">
         <v>30</v>
       </c>
@@ -4257,14 +4219,14 @@
         <v>29</v>
       </c>
       <c r="C70" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D70" s="29"/>
       <c r="E70" s="29"/>
       <c r="F70" s="29"/>
       <c r="G70" s="29"/>
       <c r="H70" s="29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I70" s="29" t="s">
         <v>21</v>
@@ -4273,7 +4235,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" s="19" t="s">
         <v>30</v>
       </c>
@@ -4281,14 +4243,14 @@
         <v>29</v>
       </c>
       <c r="C71" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D71" s="29"/>
       <c r="E71" s="29"/>
       <c r="F71" s="29"/>
       <c r="G71" s="29"/>
       <c r="H71" s="29" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I71" s="29" t="s">
         <v>20</v>
@@ -4297,7 +4259,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" s="19" t="s">
         <v>30</v>
       </c>
@@ -4305,14 +4267,14 @@
         <v>29</v>
       </c>
       <c r="C72" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D72" s="29"/>
       <c r="E72" s="29"/>
       <c r="F72" s="29"/>
       <c r="G72" s="29"/>
       <c r="H72" s="29" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I72" s="29" t="s">
         <v>20</v>
@@ -4321,7 +4283,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" s="19" t="s">
         <v>30</v>
       </c>
@@ -4343,7 +4305,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" s="19" t="s">
         <v>30</v>
       </c>

</xml_diff>